<commit_message>
test update, README.md added
</commit_message>
<xml_diff>
--- a/Чек-Лист.xlsx
+++ b/Чек-Лист.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaProjects\RelexQATest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BAAC7E0-9584-4171-B34F-861E5135A563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F29E23C5-EFA4-45E4-8A38-CE578481D8F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12765" yWindow="2955" windowWidth="21600" windowHeight="11385" xr2:uid="{43209D28-7B8D-41F5-B62C-3F37BB8C303E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{43209D28-7B8D-41F5-B62C-3F37BB8C303E}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="100">
   <si>
     <t>№Теста</t>
   </si>
@@ -328,6 +328,12 @@
   </si>
   <si>
     <t>Пользователь удаляет другого существующего пользователя</t>
+  </si>
+  <si>
+    <t>Примечание</t>
+  </si>
+  <si>
+    <t>Можно создать имя, состоящее из одной буквы</t>
   </si>
 </sst>
 </file>
@@ -358,7 +364,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -377,8 +383,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="25">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -411,8 +423,25 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="medium">
@@ -430,7 +459,48 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -439,7 +509,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -448,19 +518,34 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -472,166 +557,7 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -669,7 +595,163 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="medium">
@@ -677,45 +759,6 @@
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -724,7 +767,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -732,239 +775,254 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1279,10 +1337,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57A2AF59-0E39-48C1-8EBF-090070F91C6A}">
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:XFD33"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1294,577 +1352,631 @@
     <col min="5" max="5" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="58" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="74" t="s">
+      <c r="E1" s="81" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="49" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="75"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="76"/>
-    </row>
-    <row r="3" spans="1:4" s="38" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="34" t="s">
+      <c r="B2" s="93"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="82"/>
+    </row>
+    <row r="3" spans="1:5" s="84" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="37" t="s">
+      <c r="D3" s="59" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="16"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="74" t="s">
+      <c r="E3" s="83"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="78"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="92" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="75"/>
-      <c r="C5" s="75"/>
-      <c r="D5" s="76"/>
-    </row>
-    <row r="6" spans="1:4" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="39" t="s">
+      <c r="B5" s="93"/>
+      <c r="C5" s="93"/>
+      <c r="D5" s="94"/>
+      <c r="E5" s="78"/>
+    </row>
+    <row r="6" spans="1:5" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="41" t="s">
+      <c r="C6" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="42" t="s">
+      <c r="D6" s="60" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="44" t="s">
+      <c r="E6" s="85"/>
+    </row>
+    <row r="7" spans="1:5" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="46" t="s">
+      <c r="C7" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="47" t="s">
+      <c r="D7" s="61" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="44" t="s">
+      <c r="E7" s="85"/>
+    </row>
+    <row r="8" spans="1:5" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="45" t="s">
+      <c r="B8" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="46" t="s">
+      <c r="C8" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="47" t="s">
+      <c r="D8" s="61" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" s="43" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="48" t="s">
+      <c r="E8" s="85"/>
+    </row>
+    <row r="9" spans="1:5" s="86" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="49" t="s">
+      <c r="B9" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="50" t="s">
+      <c r="C9" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="51" t="s">
+      <c r="D9" s="62" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="77" t="s">
+      <c r="E9" s="85"/>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E10" s="78"/>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="95" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="78"/>
-      <c r="C11" s="78"/>
-      <c r="D11" s="79"/>
-    </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="59" t="s">
+      <c r="B11" s="96"/>
+      <c r="C11" s="96"/>
+      <c r="D11" s="97"/>
+      <c r="E11" s="78"/>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="60" t="s">
+      <c r="B12" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="61" t="s">
+      <c r="C12" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="62" t="s">
+      <c r="D12" s="63" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" s="43" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="52" t="s">
+      <c r="E12" s="78"/>
+    </row>
+    <row r="13" spans="1:5" s="86" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="53" t="s">
+      <c r="B13" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="63" t="s">
+      <c r="C13" s="40" t="s">
         <v>24</v>
       </c>
       <c r="D13" s="64" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" s="43" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="65" t="s">
+      <c r="E13" s="85"/>
+    </row>
+    <row r="14" spans="1:5" s="86" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="66" t="s">
+      <c r="B14" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="80" t="s">
+      <c r="C14" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="81" t="s">
+      <c r="D14" s="65" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="77" t="s">
+      <c r="E14" s="85"/>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E15" s="78"/>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="98" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="78"/>
-      <c r="C16" s="78"/>
-      <c r="D16" s="79"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
+      <c r="B16" s="99"/>
+      <c r="C16" s="99"/>
+      <c r="D16" s="100"/>
+      <c r="E16" s="78"/>
+    </row>
+    <row r="17" spans="1:5" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15" t="s">
+      <c r="B17" s="24"/>
+      <c r="C17" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="25"/>
-    </row>
-    <row r="18" spans="1:4" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="44" t="s">
+      <c r="D17" s="66"/>
+      <c r="E17" s="85"/>
+    </row>
+    <row r="18" spans="1:5" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="45" t="s">
+      <c r="B18" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="56" t="s">
+      <c r="C18" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="55" t="s">
+      <c r="D18" s="67" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
+      <c r="E18" s="85"/>
+    </row>
+    <row r="19" spans="1:5" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="12"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
+      <c r="D19" s="68"/>
+      <c r="E19" s="85"/>
+    </row>
+    <row r="20" spans="1:5" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="67" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
+      <c r="E20" s="85"/>
+    </row>
+    <row r="21" spans="1:5" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D21" s="67" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
+      <c r="E21" s="85"/>
+    </row>
+    <row r="22" spans="1:5" s="86" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="57" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D22" s="69" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
+      <c r="E22" s="79" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="D23" s="67" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
+      <c r="E23" s="85"/>
+    </row>
+    <row r="24" spans="1:5" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="D24" s="67" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
+      <c r="E24" s="85"/>
+    </row>
+    <row r="25" spans="1:5" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="D25" s="12" t="s">
+      <c r="D25" s="67" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="13" t="s">
+      <c r="E25" s="85"/>
+    </row>
+    <row r="26" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="23" t="s">
+      <c r="C26" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="D26" s="24" t="s">
+      <c r="D26" s="89" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="71"/>
-      <c r="B27" s="72"/>
-      <c r="C27" s="72"/>
-      <c r="D27" s="73"/>
-    </row>
-    <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="29" t="s">
+      <c r="E26" s="85"/>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="90"/>
+      <c r="B27" s="91"/>
+      <c r="C27" s="91"/>
+      <c r="D27" s="91"/>
+      <c r="E27" s="85"/>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="B28" s="30"/>
-      <c r="C28" s="4" t="s">
+      <c r="B28" s="18"/>
+      <c r="C28" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D28" s="31"/>
-    </row>
-    <row r="29" spans="1:4" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="39" t="s">
+      <c r="D28" s="71"/>
+      <c r="E28" s="85"/>
+    </row>
+    <row r="29" spans="1:5" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="B29" s="60" t="s">
+      <c r="B29" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="C29" s="69" t="s">
+      <c r="C29" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="D29" s="70" t="s">
+      <c r="D29" s="66" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="19" t="s">
+      <c r="E29" s="85"/>
+    </row>
+    <row r="30" spans="1:5" s="86" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="B30" s="18" t="s">
+      <c r="B30" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="C30" s="22" t="s">
+      <c r="C30" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="D30" s="20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" s="43" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="52" t="s">
+      <c r="D30" s="64" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30" s="85"/>
+    </row>
+    <row r="31" spans="1:5" s="86" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="B31" s="53" t="s">
+      <c r="B31" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="C31" s="54" t="s">
+      <c r="C31" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="D31" s="55" t="s">
+      <c r="D31" s="67" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" s="86" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="82" t="s">
+      <c r="E31" s="85"/>
+    </row>
+    <row r="32" spans="1:5" s="49" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="B32" s="83" t="s">
+      <c r="B32" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="C32" s="84" t="s">
+      <c r="C32" s="48" t="s">
         <v>74</v>
       </c>
-      <c r="D32" s="85" t="s">
+      <c r="D32" s="72" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" s="91" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="87" t="s">
+      <c r="E32" s="85"/>
+    </row>
+    <row r="33" spans="1:5" s="88" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="50" t="s">
         <v>75</v>
       </c>
-      <c r="B33" s="88" t="s">
+      <c r="B33" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="C33" s="89" t="s">
+      <c r="C33" s="52" t="s">
         <v>76</v>
       </c>
-      <c r="D33" s="90" t="s">
+      <c r="D33" s="73" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="71"/>
-      <c r="B34" s="72"/>
-      <c r="C34" s="72"/>
-      <c r="D34" s="73"/>
-    </row>
-    <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="29" t="s">
+      <c r="E33" s="87"/>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="90"/>
+      <c r="B34" s="91"/>
+      <c r="C34" s="91"/>
+      <c r="D34" s="91"/>
+      <c r="E34" s="85"/>
+    </row>
+    <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="B35" s="30"/>
-      <c r="C35" s="4" t="s">
+      <c r="B35" s="18"/>
+      <c r="C35" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D35" s="31"/>
-    </row>
-    <row r="36" spans="1:4" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="39" t="s">
+      <c r="D35" s="71"/>
+      <c r="E35" s="85"/>
+    </row>
+    <row r="36" spans="1:5" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="B36" s="60" t="s">
+      <c r="B36" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="C36" s="69" t="s">
+      <c r="C36" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="D36" s="70" t="s">
+      <c r="D36" s="66" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="19" t="s">
+      <c r="E36" s="85"/>
+    </row>
+    <row r="37" spans="1:5" s="86" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="B37" s="18" t="s">
+      <c r="B37" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="22" t="s">
+      <c r="C37" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="D37" s="20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="19" t="s">
+      <c r="D37" s="64" t="s">
+        <v>27</v>
+      </c>
+      <c r="E37" s="85"/>
+    </row>
+    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="B38" s="18" t="s">
+      <c r="B38" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="C38" s="22" t="s">
+      <c r="C38" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="D38" s="32" t="s">
+      <c r="D38" s="74" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" s="43" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="52" t="s">
+      <c r="E38" s="85"/>
+    </row>
+    <row r="39" spans="1:5" s="86" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="B39" s="53" t="s">
+      <c r="B39" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="C39" s="57" t="s">
+      <c r="C39" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="D39" s="58" t="s">
+      <c r="D39" s="74" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" s="43" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="65" t="s">
+      <c r="E39" s="85"/>
+    </row>
+    <row r="40" spans="1:5" s="86" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="B40" s="66" t="s">
+      <c r="B40" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="C40" s="67" t="s">
+      <c r="C40" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="D40" s="68" t="s">
+      <c r="D40" s="75" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="71"/>
-      <c r="B41" s="72"/>
-      <c r="C41" s="72"/>
-      <c r="D41" s="73"/>
-    </row>
-    <row r="42" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="29" t="s">
+      <c r="E40" s="85"/>
+    </row>
+    <row r="41" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="90"/>
+      <c r="B41" s="91"/>
+      <c r="C41" s="91"/>
+      <c r="D41" s="91"/>
+      <c r="E41" s="85"/>
+    </row>
+    <row r="42" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="B42" s="30"/>
-      <c r="C42" s="4" t="s">
+      <c r="B42" s="18"/>
+      <c r="C42" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D42" s="31"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="26" t="s">
+      <c r="D42" s="71"/>
+      <c r="E42" s="85"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="B43" s="27" t="s">
+      <c r="B43" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="C43" s="33" t="s">
+      <c r="C43" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="D43" s="28" t="s">
+      <c r="D43" s="76" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="14" t="s">
+      <c r="E43" s="85"/>
+    </row>
+    <row r="44" spans="1:5" s="86" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="B44" s="18" t="s">
+      <c r="B44" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="C44" s="22" t="s">
+      <c r="C44" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="D44" s="20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="14" t="s">
+      <c r="D44" s="64" t="s">
+        <v>27</v>
+      </c>
+      <c r="E44" s="85"/>
+    </row>
+    <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="B45" s="18" t="s">
+      <c r="B45" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="C45" s="22" t="s">
+      <c r="C45" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="D45" s="12" t="s">
+      <c r="D45" s="77" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="14" t="s">
+      <c r="E45" s="85"/>
+    </row>
+    <row r="46" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="B46" s="18" t="s">
+      <c r="B46" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="C46" s="22" t="s">
+      <c r="C46" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="D46" s="12" t="s">
+      <c r="D46" s="77" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="14" t="s">
+      <c r="E46" s="85"/>
+    </row>
+    <row r="47" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="B47" s="18" t="s">
+      <c r="B47" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="C47" s="22" t="s">
+      <c r="C47" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="D47" s="12" t="s">
+      <c r="D47" s="77" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="17" t="s">
+      <c r="E47" s="78"/>
+    </row>
+    <row r="48" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="B48" s="21" t="s">
+      <c r="B48" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="C48" s="23" t="s">
+      <c r="C48" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="D48" s="24" t="s">
+      <c r="D48" s="70" t="s">
         <v>53</v>
       </c>
+      <c r="E48" s="80"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>